<commit_message>
GeneralViewModel ve PartialAdd ayarlandı list hazırlanacak
</commit_message>
<xml_diff>
--- a/Kariyer Masası.xlsx
+++ b/Kariyer Masası.xlsx
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
       <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I1" t="s">
@@ -600,7 +600,7 @@
       <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -635,7 +635,7 @@
       <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" t="s">
@@ -647,7 +647,7 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="1" t="s">

</xml_diff>